<commit_message>
整理文件 Signed-off-by: anshu.wang <anshu.wang.work@gmail.com>
</commit_message>
<xml_diff>
--- a/writting/学科知识体系/教育学/足球情报收集.xlsx
+++ b/writting/学科知识体系/教育学/足球情报收集.xlsx
@@ -4,17 +4,18 @@
   <fileVersion appName="xl" lastEdited="3" lowestEdited="5" rupBuild="9302"/>
   <workbookPr/>
   <bookViews>
-    <workbookView windowWidth="21495" windowHeight="11385"/>
+    <workbookView windowWidth="22943" windowHeight="9804" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
+    <sheet name="Sheet2" sheetId="2" r:id="rId2"/>
   </sheets>
   <calcPr calcId="144525"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="19">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="26">
   <si>
     <t>windrawwin.com</t>
   </si>
@@ -71,6 +72,27 @@
   </si>
   <si>
     <t>http://fcstats.com/statistics,premier-league-england,1,5,1938.php</t>
+  </si>
+  <si>
+    <t>分析赛事所有因素</t>
+  </si>
+  <si>
+    <t>耗费时间长，压力大</t>
+  </si>
+  <si>
+    <t>综合数据</t>
+  </si>
+  <si>
+    <t>大小球</t>
+  </si>
+  <si>
+    <t>赛事少</t>
+  </si>
+  <si>
+    <t>高赔率，双胜彩</t>
+  </si>
+  <si>
+    <t>赔率低，稳定</t>
   </si>
 </sst>
 </file>
@@ -78,10 +100,10 @@
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <numFmts count="4">
-    <numFmt numFmtId="176" formatCode="_ \￥* #,##0.00_ ;_ \￥* \-#,##0.00_ ;_ \￥* &quot;-&quot;??_ ;_ @_ "/>
     <numFmt numFmtId="43" formatCode="_ * #,##0.00_ ;_ * \-#,##0.00_ ;_ * &quot;-&quot;??_ ;_ @_ "/>
     <numFmt numFmtId="41" formatCode="_ * #,##0_ ;_ * \-#,##0_ ;_ * &quot;-&quot;_ ;_ @_ "/>
-    <numFmt numFmtId="177" formatCode="_ \￥* #,##0_ ;_ \￥* \-#,##0_ ;_ \￥* &quot;-&quot;_ ;_ @_ "/>
+    <numFmt numFmtId="176" formatCode="_ \￥* #,##0_ ;_ \￥* \-#,##0_ ;_ \￥* &quot;-&quot;_ ;_ @_ "/>
+    <numFmt numFmtId="177" formatCode="_ \￥* #,##0.00_ ;_ \￥* \-#,##0.00_ ;_ \￥* &quot;-&quot;??_ ;_ @_ "/>
   </numFmts>
   <fonts count="20">
     <font>
@@ -109,6 +131,28 @@
     </font>
     <font>
       <sz val="11"/>
+      <color rgb="FFFF0000"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <i/>
+      <sz val="11"/>
+      <color rgb="FF7F7F7F"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
       <color theme="0"/>
       <name val="Calibri"/>
       <charset val="0"/>
@@ -116,9 +160,41 @@
     </font>
     <font>
       <sz val="11"/>
-      <color theme="1"/>
+      <color rgb="FF3F3F76"/>
       <name val="Calibri"/>
       <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="13"/>
+      <color theme="3"/>
+      <name val="Calibri"/>
+      <charset val="134"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color rgb="FFFA7D00"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color rgb="FFFFFFFF"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="15"/>
+      <color theme="3"/>
+      <name val="Calibri"/>
+      <charset val="134"/>
       <scheme val="minor"/>
     </font>
     <font>
@@ -130,100 +206,46 @@
       <scheme val="minor"/>
     </font>
     <font>
+      <sz val="11"/>
+      <color rgb="FF9C0006"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
       <b/>
       <sz val="11"/>
+      <color theme="3"/>
+      <name val="Calibri"/>
+      <charset val="134"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
       <color theme="1"/>
       <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
     </font>
     <font>
+      <sz val="11"/>
+      <color rgb="FFFA7D00"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF006100"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
       <b/>
-      <sz val="13"/>
-      <color theme="3"/>
-      <name val="Calibri"/>
-      <charset val="134"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <i/>
-      <sz val="11"/>
-      <color rgb="FF7F7F7F"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="11"/>
-      <color rgb="FFFFFFFF"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FFFF0000"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FF9C0006"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FFFA7D00"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="15"/>
-      <color theme="3"/>
-      <name val="Calibri"/>
-      <charset val="134"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FF006100"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="11"/>
-      <color theme="3"/>
-      <name val="Calibri"/>
-      <charset val="134"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FF3F3F76"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
       <sz val="11"/>
       <color rgb="FF3F3F3F"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="11"/>
-      <color rgb="FFFA7D00"/>
       <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
@@ -245,13 +267,97 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFCC99"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFF2F2F2"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFA5A5A5"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
         <fgColor theme="8" tint="0.399975585192419"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.399975585192419"/>
+        <fgColor theme="8"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFFFCC"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -263,13 +369,55 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="7"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8"/>
+        <fgColor theme="6" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFC7CE"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFC6EFCE"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -287,145 +435,19 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor rgb="FFFFFFCC"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFA5A5A5"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFC7CE"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFC6EFCE"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFCC99"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFF2F2F2"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.799981688894314"/>
+        <fgColor theme="4"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFEB9C"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
         <fgColor theme="4" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFEB9C"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.799981688894314"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -440,27 +462,16 @@
     </border>
     <border>
       <left style="thin">
-        <color rgb="FFB2B2B2"/>
+        <color rgb="FF7F7F7F"/>
       </left>
       <right style="thin">
-        <color rgb="FFB2B2B2"/>
+        <color rgb="FF7F7F7F"/>
       </right>
       <top style="thin">
-        <color rgb="FFB2B2B2"/>
+        <color rgb="FF7F7F7F"/>
       </top>
       <bottom style="thin">
-        <color rgb="FFB2B2B2"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left/>
-      <right/>
-      <top style="thin">
-        <color theme="4"/>
-      </top>
-      <bottom style="double">
-        <color theme="4"/>
+        <color rgb="FF7F7F7F"/>
       </bottom>
       <diagonal/>
     </border>
@@ -489,11 +500,17 @@
       <diagonal/>
     </border>
     <border>
-      <left/>
-      <right/>
-      <top/>
-      <bottom style="double">
-        <color rgb="FFFF8001"/>
+      <left style="thin">
+        <color rgb="FFB2B2B2"/>
+      </left>
+      <right style="thin">
+        <color rgb="FFB2B2B2"/>
+      </right>
+      <top style="thin">
+        <color rgb="FFB2B2B2"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="FFB2B2B2"/>
       </bottom>
       <diagonal/>
     </border>
@@ -507,17 +524,22 @@
       <diagonal/>
     </border>
     <border>
-      <left style="thin">
-        <color rgb="FF7F7F7F"/>
-      </left>
-      <right style="thin">
-        <color rgb="FF7F7F7F"/>
-      </right>
+      <left/>
+      <right/>
       <top style="thin">
-        <color rgb="FF7F7F7F"/>
+        <color theme="4"/>
       </top>
-      <bottom style="thin">
-        <color rgb="FF7F7F7F"/>
+      <bottom style="double">
+        <color theme="4"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top/>
+      <bottom style="double">
+        <color rgb="FFFF8001"/>
       </bottom>
       <diagonal/>
     </border>
@@ -541,7 +563,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="12" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="5" fillId="16" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="43" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
@@ -550,139 +572,139 @@
     <xf numFmtId="41" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
+    <xf numFmtId="176" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
     <xf numFmtId="177" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="176" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
     <xf numFmtId="9" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="9" fillId="14" borderId="4" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="3" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="9" borderId="1" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="10" fillId="12" borderId="3" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="2" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="17" borderId="4" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="11" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="6" fillId="21" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="16" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="19" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="0" borderId="3" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="5" fillId="11" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="6" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="2" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="0" borderId="5" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="5" borderId="1" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="4" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="17" fillId="24" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="18" fillId="10" borderId="8" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="10" borderId="1" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="16" fillId="0" borderId="7" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="15" fillId="0" borderId="6" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="15" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="16" fillId="21" borderId="7" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="3" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="14" fillId="20" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="17" fillId="22" borderId="8" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="24" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="18" fillId="22" borderId="7" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="0" borderId="5" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="2" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="18" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="19" fillId="27" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="29" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="17" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="30" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="8" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="26" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="28" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="23" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="5" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="7" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="10" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="6" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="15" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="2" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="4" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="25" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="13" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="13" fillId="20" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="19" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="30" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="3" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="23" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="27" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="15" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="29" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="22" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="26" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="19" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="9" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="28" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="2" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="14" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="8" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="13" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="18" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="7" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="25" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
   </cellStyleXfs>
@@ -787,8 +809,8 @@
       </xdr:blipFill>
       <xdr:spPr>
         <a:xfrm>
-          <a:off x="3743325" y="7239000"/>
-          <a:ext cx="304800" cy="304800"/>
+          <a:off x="3851275" y="6949440"/>
+          <a:ext cx="304800" cy="297180"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -829,8 +851,8 @@
       </xdr:blipFill>
       <xdr:spPr>
         <a:xfrm>
-          <a:off x="30480" y="10134600"/>
-          <a:ext cx="4999990" cy="2790190"/>
+          <a:off x="30480" y="9730740"/>
+          <a:ext cx="5142230" cy="2683510"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -871,8 +893,8 @@
       </xdr:blipFill>
       <xdr:spPr>
         <a:xfrm>
-          <a:off x="6200775" y="10077450"/>
-          <a:ext cx="5552440" cy="3142615"/>
+          <a:off x="6377305" y="9681210"/>
+          <a:ext cx="5706745" cy="3013075"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -913,8 +935,8 @@
       </xdr:blipFill>
       <xdr:spPr>
         <a:xfrm>
-          <a:off x="230505" y="4438650"/>
-          <a:ext cx="5152390" cy="4609465"/>
+          <a:off x="230505" y="4263390"/>
+          <a:ext cx="5294630" cy="4426585"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -955,8 +977,8 @@
       </xdr:blipFill>
       <xdr:spPr>
         <a:xfrm>
-          <a:off x="6189980" y="4505325"/>
-          <a:ext cx="5200015" cy="4523740"/>
+          <a:off x="6366510" y="4330065"/>
+          <a:ext cx="5337175" cy="4340860"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -997,8 +1019,8 @@
       </xdr:blipFill>
       <xdr:spPr>
         <a:xfrm>
-          <a:off x="11445240" y="4381500"/>
-          <a:ext cx="5257165" cy="4723765"/>
+          <a:off x="11776075" y="4206240"/>
+          <a:ext cx="5394325" cy="4540885"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -1039,8 +1061,8 @@
       </xdr:blipFill>
       <xdr:spPr>
         <a:xfrm>
-          <a:off x="4335780" y="14287500"/>
-          <a:ext cx="4933315" cy="6304915"/>
+          <a:off x="4460875" y="13716000"/>
+          <a:ext cx="5070475" cy="6053455"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -1316,13 +1338,13 @@
   <sheetPr/>
   <dimension ref="A1:K74"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A7" workbookViewId="0">
+    <sheetView topLeftCell="A7" workbookViewId="0">
       <selection activeCell="H17" sqref="H17"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.88571428571429" defaultRowHeight="15"/>
+  <sheetFormatPr defaultColWidth="8.88888888888889" defaultRowHeight="14.4"/>
   <cols>
-    <col min="4" max="4" width="11.7142857142857" customWidth="1"/>
+    <col min="4" max="4" width="11.712962962963" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:4">
@@ -1432,4 +1454,56 @@
   <headerFooter/>
   <drawing r:id="rId1"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:etc="http://www.wps.cn/officeDocument/2017/etCustomData">
+  <sheetPr/>
+  <dimension ref="B3:C6"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="B7" sqref="B7"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultColWidth="8.88888888888889" defaultRowHeight="14.4" outlineLevelRow="5" outlineLevelCol="2"/>
+  <cols>
+    <col min="2" max="2" width="18.6666666666667" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="3" spans="2:3">
+      <c r="B3" t="s">
+        <v>19</v>
+      </c>
+      <c r="C3" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="4" spans="2:3">
+      <c r="B4" t="s">
+        <v>21</v>
+      </c>
+      <c r="C4" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="5" spans="2:3">
+      <c r="B5" t="s">
+        <v>22</v>
+      </c>
+      <c r="C5" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="6" spans="2:3">
+      <c r="B6" t="s">
+        <v>24</v>
+      </c>
+      <c r="C6" t="s">
+        <v>25</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.511805555555556" footer="0.511805555555556"/>
+  <headerFooter/>
+</worksheet>
 </file>
</xml_diff>